<commit_message>
fix: reorder eventDistance assignment in lookup patterns for clarity
</commit_message>
<xml_diff>
--- a/doc/mappings.xlsx
+++ b/doc/mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\src\zwift-memory-monitor\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\zwift-memory-monitor\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB1D9DD-D0A3-4F56-AA7B-F57A0A6BF3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430CCBB0-4792-4923-8683-45DF40AEB8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="825" windowWidth="34305" windowHeight="18915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.29.0" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="241">
   <si>
     <t>Type</t>
   </si>
@@ -256,9 +256,6 @@
     <t>protobuf field no.</t>
   </si>
   <si>
-    <t>LAPS??</t>
-  </si>
-  <si>
     <t>export function decodePlayerStateFlags1(bits) {</t>
   </si>
   <si>
@@ -733,9 +730,6 @@
     <t>TO BE ADDED TO ZMM - roadid, activepowerup</t>
   </si>
   <si>
-    <t>DRAFT?</t>
-  </si>
-  <si>
     <t>! F19</t>
   </si>
   <si>
@@ -743,6 +737,33 @@
   </si>
   <si>
     <t>! CourseID</t>
+  </si>
+  <si>
+    <t>uint64</t>
+  </si>
+  <si>
+    <t>laps</t>
+  </si>
+  <si>
+    <t>draft</t>
+  </si>
+  <si>
+    <t>eventDistance</t>
+  </si>
+  <si>
+    <t>checkPointId</t>
+  </si>
+  <si>
+    <t>gradientScale</t>
+  </si>
+  <si>
+    <t>elevationScalePct</t>
+  </si>
+  <si>
+    <t>// 50, 75, 100, 125</t>
+  </si>
+  <si>
+    <t>// 0 ~ 50%, 1 ~ 75%, 2 ~ 100%, 3 ~ 125%</t>
   </si>
 </sst>
 </file>
@@ -1103,24 +1124,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z70"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="5"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" style="5"/>
+    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="5" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="5" customWidth="1"/>
-    <col min="5" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" style="5" customWidth="1"/>
+    <col min="5" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="29.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4">
         <v>0</v>
       </c>
@@ -1149,7 +1170,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -1158,15 +1179,15 @@
         <v>0x0</v>
       </c>
       <c r="C2" s="5" t="str">
-        <f>IF((A2-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A2-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f>"0x"&amp;DEC2HEX(D2)</f>
         <v>0x0</v>
       </c>
       <c r="D2" s="5">
-        <f>(A2-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" ref="D2:D33" si="1">(A2-INDEX(A:A,MATCH("player",F:F,0)))</f>
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>232</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -1178,9 +1199,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
-        <f t="shared" ref="A3:A59" si="1">A2+4</f>
+        <f t="shared" ref="A3:A59" si="2">A2+4</f>
         <v>4</v>
       </c>
       <c r="B3" t="str">
@@ -1188,33 +1209,36 @@
         <v>0x4</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f>IF((A3-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A3-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" ref="C3:C66" si="3">"0x"&amp;DEC2HEX(D3)</f>
         <v>0x4</v>
       </c>
       <c r="D3" s="5">
-        <f>(A3-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>0x8</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x8</v>
+      </c>
+      <c r="D4" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>0x8</v>
-      </c>
-      <c r="C4" s="5" t="str">
-        <f>IF((A4-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A4-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x8</v>
-      </c>
-      <c r="D4" s="5">
-        <f>(A4-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>8</v>
+      <c r="E4" t="s">
+        <v>4</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -1223,41 +1247,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>0xC</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0xC</v>
+      </c>
+      <c r="D5" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>0xC</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <f>IF((A5-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A5-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x12</v>
-      </c>
-      <c r="D5" s="5">
-        <f>(A5-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x10</v>
+      </c>
+      <c r="D6" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>0x10</v>
-      </c>
-      <c r="C6" s="5" t="str">
-        <f>IF((A6-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A6-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x16</v>
-      </c>
-      <c r="D6" s="5">
-        <f>(A6-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>16</v>
-      </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -1271,23 +1295,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x14</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x14</v>
+      </c>
+      <c r="D7" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>0x14</v>
-      </c>
-      <c r="C7" s="5" t="str">
-        <f>IF((A7-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A7-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x20</v>
-      </c>
-      <c r="D7" s="5">
-        <f>(A7-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>20</v>
-      </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
@@ -1301,47 +1325,53 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>0x18</v>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x18</v>
+      </c>
+      <c r="D8" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>0x18</v>
-      </c>
-      <c r="C8" s="5" t="str">
-        <f>IF((A8-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A8-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x24</v>
-      </c>
-      <c r="D8" s="5">
-        <f>(A8-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>24</v>
-      </c>
-      <c r="I8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>233</v>
+      </c>
+      <c r="G8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>0x1C</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x1C</v>
+      </c>
+      <c r="D9" s="5">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>0x1C</v>
-      </c>
-      <c r="C9" s="5" t="str">
-        <f>IF((A9-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A9-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x28</v>
-      </c>
-      <c r="D9" s="5">
-        <f>(A9-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>28</v>
-      </c>
       <c r="E9" t="s">
         <v>4</v>
       </c>
@@ -1355,62 +1385,62 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>0x20</v>
+      </c>
+      <c r="C10" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x20</v>
+      </c>
+      <c r="D10" s="5">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>0x20</v>
-      </c>
-      <c r="C10" s="5" t="str">
-        <f>IF((A10-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A10-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x32</v>
-      </c>
-      <c r="D10" s="5">
-        <f>(A10-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>0x24</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x24</v>
+      </c>
+      <c r="D11" s="5">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>0x24</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <f>IF((A11-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A11-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x36</v>
-      </c>
-      <c r="D11" s="5">
-        <f>(A11-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>36</v>
-      </c>
       <c r="J11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>0x28</v>
+      </c>
+      <c r="C12" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x28</v>
+      </c>
+      <c r="D12" s="5">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>0x28</v>
-      </c>
-      <c r="C12" s="5" t="str">
-        <f>IF((A12-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A12-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x40</v>
-      </c>
-      <c r="D12" s="5">
-        <f>(A12-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>40</v>
-      </c>
       <c r="E12" t="s">
         <v>4</v>
       </c>
@@ -1424,47 +1454,53 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>0x2C</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x2C</v>
+      </c>
+      <c r="D13" s="5">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>0x2C</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <f>IF((A13-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A13-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x44</v>
-      </c>
-      <c r="D13" s="5">
-        <f>(A13-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>44</v>
-      </c>
-      <c r="I13" t="s">
-        <v>230</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>234</v>
+      </c>
+      <c r="G13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>0x30</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x30</v>
+      </c>
+      <c r="D14" s="5">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>0x30</v>
-      </c>
-      <c r="C14" s="5" t="str">
-        <f>IF((A14-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A14-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x48</v>
-      </c>
-      <c r="D14" s="5">
-        <f>(A14-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>48</v>
-      </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
@@ -1478,23 +1514,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>0x34</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x34</v>
+      </c>
+      <c r="D15" s="5">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>0x34</v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <f>IF((A15-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A15-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x52</v>
-      </c>
-      <c r="D15" s="5">
-        <f>(A15-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>52</v>
-      </c>
       <c r="E15" t="s">
         <v>4</v>
       </c>
@@ -1508,65 +1544,65 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>0x38</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x38</v>
+      </c>
+      <c r="D16" s="5">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>0x38</v>
-      </c>
-      <c r="C16" s="5" t="str">
-        <f>IF((A16-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A16-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x56</v>
-      </c>
-      <c r="D16" s="5">
-        <f>(A16-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>56</v>
-      </c>
       <c r="J16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>0x3C</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x3C</v>
+      </c>
+      <c r="D17" s="5">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>0x3C</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <f>IF((A17-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A17-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x60</v>
-      </c>
-      <c r="D17" s="5">
-        <f>(A17-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>60</v>
-      </c>
       <c r="J17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>0x40</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x40</v>
+      </c>
+      <c r="D18" s="5">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>0x40</v>
-      </c>
-      <c r="C18" s="5" t="str">
-        <f>IF((A18-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A18-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x64</v>
-      </c>
-      <c r="D18" s="5">
-        <f>(A18-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>64</v>
-      </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
@@ -1580,23 +1616,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>0x44</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x44</v>
+      </c>
+      <c r="D19" s="5">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>0x44</v>
-      </c>
-      <c r="C19" s="5" t="str">
-        <f>IF((A19-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A19-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x68</v>
-      </c>
-      <c r="D19" s="5">
-        <f>(A19-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>68</v>
-      </c>
       <c r="E19" t="s">
         <v>4</v>
       </c>
@@ -1610,185 +1646,185 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>0x48</v>
+      </c>
+      <c r="C20" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x48</v>
+      </c>
+      <c r="D20" s="5">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>0x48</v>
-      </c>
-      <c r="C20" s="5" t="str">
-        <f>IF((A20-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A20-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x72</v>
-      </c>
-      <c r="D20" s="5">
-        <f>(A20-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x4C</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x4C</v>
+      </c>
+      <c r="D21" s="5">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>0x4C</v>
-      </c>
-      <c r="C21" s="5" t="str">
-        <f>IF((A21-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A21-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x76</v>
-      </c>
-      <c r="D21" s="5">
-        <f>(A21-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>76</v>
-      </c>
       <c r="O21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>0x50</v>
+      </c>
+      <c r="C22" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x50</v>
+      </c>
+      <c r="D22" s="5">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>0x50</v>
-      </c>
-      <c r="C22" s="5" t="str">
-        <f>IF((A22-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A22-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x80</v>
-      </c>
-      <c r="D22" s="5">
-        <f>(A22-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>80</v>
-      </c>
       <c r="F22" t="s">
+        <v>226</v>
+      </c>
+      <c r="I22" t="s">
+        <v>229</v>
+      </c>
+      <c r="J22" t="s">
         <v>227</v>
-      </c>
-      <c r="I22" t="s">
-        <v>231</v>
-      </c>
-      <c r="J22" t="s">
-        <v>228</v>
       </c>
       <c r="O22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>0x54</v>
+      </c>
+      <c r="C23" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x54</v>
+      </c>
+      <c r="D23" s="5">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v>0x54</v>
-      </c>
-      <c r="C23" s="5" t="str">
-        <f>IF((A23-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A23-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x84</v>
-      </c>
-      <c r="D23" s="5">
-        <f>(A23-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>84</v>
-      </c>
       <c r="F23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I23" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>0x58</v>
+      </c>
+      <c r="C24" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x58</v>
+      </c>
+      <c r="D24" s="5">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>0x58</v>
-      </c>
-      <c r="C24" s="5" t="str">
-        <f>IF((A24-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A24-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x88</v>
-      </c>
-      <c r="D24" s="5">
-        <f>(A24-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="O24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x5C</v>
+      </c>
+      <c r="C25" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x5C</v>
+      </c>
+      <c r="D25" s="5">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>0x5C</v>
-      </c>
-      <c r="C25" s="5" t="str">
-        <f>IF((A25-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A25-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x92</v>
-      </c>
-      <c r="D25" s="5">
-        <f>(A25-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>92</v>
-      </c>
-      <c r="Z25" t="s">
+      <c r="O25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>0x60</v>
+      </c>
+      <c r="C26" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x60</v>
+      </c>
+      <c r="D26" s="5">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>0x60</v>
-      </c>
-      <c r="C26" s="5" t="str">
-        <f>IF((A26-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A26-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x96</v>
-      </c>
-      <c r="D26" s="5">
-        <f>(A26-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>96</v>
-      </c>
       <c r="O26" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>0x64</v>
+      </c>
+      <c r="C27" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x64</v>
+      </c>
+      <c r="D27" s="5">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>0x64</v>
-      </c>
-      <c r="C27" s="5" t="str">
-        <f>IF((A27-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A27-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x100</v>
-      </c>
-      <c r="D27" s="5">
-        <f>(A27-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>100</v>
-      </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
@@ -1802,23 +1838,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>0x68</v>
+      </c>
+      <c r="C28" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x68</v>
+      </c>
+      <c r="D28" s="5">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>0x68</v>
-      </c>
-      <c r="C28" s="5" t="str">
-        <f>IF((A28-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A28-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x104</v>
-      </c>
-      <c r="D28" s="5">
-        <f>(A28-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>104</v>
-      </c>
       <c r="E28" t="s">
         <v>11</v>
       </c>
@@ -1832,23 +1868,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>0x6C</v>
+      </c>
+      <c r="C29" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x6C</v>
+      </c>
+      <c r="D29" s="5">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>0x6C</v>
-      </c>
-      <c r="C29" s="5" t="str">
-        <f>IF((A29-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A29-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x108</v>
-      </c>
-      <c r="D29" s="5">
-        <f>(A29-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>108</v>
-      </c>
       <c r="E29" t="s">
         <v>11</v>
       </c>
@@ -1862,23 +1898,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>0x70</v>
+      </c>
+      <c r="C30" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x70</v>
+      </c>
+      <c r="D30" s="5">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>0x70</v>
-      </c>
-      <c r="C30" s="5" t="str">
-        <f>IF((A30-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A30-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x112</v>
-      </c>
-      <c r="D30" s="5">
-        <f>(A30-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>112</v>
-      </c>
       <c r="E30" t="s">
         <v>4</v>
       </c>
@@ -1892,41 +1928,41 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>0x74</v>
+      </c>
+      <c r="C31" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x74</v>
+      </c>
+      <c r="D31" s="5">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>0x74</v>
-      </c>
-      <c r="C31" s="5" t="str">
-        <f>IF((A31-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A31-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x116</v>
-      </c>
-      <c r="D31" s="5">
-        <f>(A31-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>0x78</v>
+      </c>
+      <c r="C32" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x78</v>
+      </c>
+      <c r="D32" s="5">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>0x78</v>
-      </c>
-      <c r="C32" s="5" t="str">
-        <f>IF((A32-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A32-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x120</v>
-      </c>
-      <c r="D32" s="5">
-        <f>(A32-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>120</v>
-      </c>
       <c r="E32" t="s">
         <v>4</v>
       </c>
@@ -1940,27 +1976,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>0x7C</v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0x7C</v>
+      </c>
+      <c r="D33" s="5">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>0x7C</v>
-      </c>
-      <c r="C33" s="5" t="str">
-        <f>IF((A33-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A33-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x124</v>
-      </c>
-      <c r="D33" s="5">
-        <f>(A33-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="B34" t="str">
@@ -1968,11 +2004,11 @@
         <v>0x80</v>
       </c>
       <c r="C34" s="5" t="str">
-        <f>IF((A34-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A34-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x128</v>
+        <f t="shared" si="3"/>
+        <v>0x80</v>
       </c>
       <c r="D34" s="5">
-        <f>(A34-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" ref="D34:D70" si="4">(A34-INDEX(A:A,MATCH("player",F:F,0)))</f>
         <v>128</v>
       </c>
       <c r="E34" t="s">
@@ -1988,9 +2024,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="B35" t="str">
@@ -1998,20 +2034,20 @@
         <v>0x84</v>
       </c>
       <c r="C35" s="5" t="str">
-        <f>IF((A35-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A35-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x132</v>
+        <f t="shared" si="3"/>
+        <v>0x84</v>
       </c>
       <c r="D35" s="5">
-        <f>(A35-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>132</v>
       </c>
       <c r="O35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>136</v>
       </c>
       <c r="B36" t="str">
@@ -2019,17 +2055,17 @@
         <v>0x88</v>
       </c>
       <c r="C36" s="5" t="str">
-        <f>IF((A36-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A36-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x136</v>
+        <f t="shared" si="3"/>
+        <v>0x88</v>
       </c>
       <c r="D36" s="5">
-        <f>(A36-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
       <c r="B37" t="str">
@@ -2037,17 +2073,17 @@
         <v>0x8C</v>
       </c>
       <c r="C37" s="5" t="str">
-        <f>IF((A37-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A37-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x140</v>
+        <f t="shared" si="3"/>
+        <v>0x8C</v>
       </c>
       <c r="D37" s="5">
-        <f>(A37-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="B38" t="str">
@@ -2055,20 +2091,26 @@
         <v>0x90</v>
       </c>
       <c r="C38" s="5" t="str">
-        <f>IF((A38-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A38-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x144</v>
+        <f t="shared" si="3"/>
+        <v>0x90</v>
       </c>
       <c r="D38" s="5">
-        <f>(A38-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>144</v>
       </c>
-      <c r="O38" t="s">
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>235</v>
+      </c>
+      <c r="G38" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="B39" t="str">
@@ -2076,18 +2118,18 @@
         <v>0x94</v>
       </c>
       <c r="C39" s="5" t="str">
-        <f>IF((A39-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A39-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x148</v>
+        <f t="shared" si="3"/>
+        <v>0x94</v>
       </c>
       <c r="D39" s="5">
-        <f>(A39-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>148</v>
       </c>
       <c r="E39" t="s">
         <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G39" t="s">
         <v>51</v>
@@ -2096,15 +2138,15 @@
         <v>35</v>
       </c>
       <c r="I39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>152</v>
       </c>
       <c r="B40" t="str">
@@ -2112,20 +2154,26 @@
         <v>0x98</v>
       </c>
       <c r="C40" s="5" t="str">
-        <f>IF((A40-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A40-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x152</v>
+        <f t="shared" si="3"/>
+        <v>0x98</v>
       </c>
       <c r="D40" s="5">
-        <f>(A40-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>152</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>236</v>
       </c>
       <c r="O40" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="B41" t="str">
@@ -2133,20 +2181,20 @@
         <v>0x9C</v>
       </c>
       <c r="C41" s="5" t="str">
-        <f>IF((A41-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A41-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x156</v>
+        <f t="shared" si="3"/>
+        <v>0x9C</v>
       </c>
       <c r="D41" s="5">
-        <f>(A41-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>156</v>
       </c>
       <c r="O41" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="B42" t="str">
@@ -2154,20 +2202,20 @@
         <v>0xA0</v>
       </c>
       <c r="C42" s="5" t="str">
-        <f>IF((A42-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A42-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x160</v>
+        <f t="shared" si="3"/>
+        <v>0xA0</v>
       </c>
       <c r="D42" s="5">
-        <f>(A42-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>160</v>
       </c>
       <c r="O42" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>164</v>
       </c>
       <c r="B43" t="str">
@@ -2175,11 +2223,11 @@
         <v>0xA4</v>
       </c>
       <c r="C43" s="5" t="str">
-        <f>IF((A43-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A43-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x164</v>
+        <f t="shared" si="3"/>
+        <v>0xA4</v>
       </c>
       <c r="D43" s="5">
-        <f>(A43-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>164</v>
       </c>
       <c r="E43" t="s">
@@ -2195,9 +2243,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>168</v>
       </c>
       <c r="B44" t="str">
@@ -2205,20 +2253,20 @@
         <v>0xA8</v>
       </c>
       <c r="C44" s="5" t="str">
-        <f>IF((A44-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A44-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x168</v>
+        <f t="shared" si="3"/>
+        <v>0xA8</v>
       </c>
       <c r="D44" s="5">
-        <f>(A44-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="O44" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>172</v>
       </c>
       <c r="B45" t="str">
@@ -2226,20 +2274,20 @@
         <v>0xAC</v>
       </c>
       <c r="C45" s="5" t="str">
-        <f>IF((A45-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A45-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x172</v>
+        <f t="shared" si="3"/>
+        <v>0xAC</v>
       </c>
       <c r="D45" s="5">
-        <f>(A45-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>172</v>
       </c>
       <c r="O45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>176</v>
       </c>
       <c r="B46" t="str">
@@ -2247,20 +2295,20 @@
         <v>0xB0</v>
       </c>
       <c r="C46" s="5" t="str">
-        <f>IF((A46-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A46-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x176</v>
+        <f t="shared" si="3"/>
+        <v>0xB0</v>
       </c>
       <c r="D46" s="5">
-        <f>(A46-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>176</v>
       </c>
       <c r="O46" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="B47" t="str">
@@ -2268,179 +2316,203 @@
         <v>0xB4</v>
       </c>
       <c r="C47" s="5" t="str">
-        <f>IF((A47-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A47-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x180</v>
+        <f t="shared" si="3"/>
+        <v>0xB4</v>
       </c>
       <c r="D47" s="5">
-        <f>(A47-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
-      <c r="O47" t="s">
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A48" s="5">
+        <f t="shared" si="2"/>
+        <v>184</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>0xB8</v>
+      </c>
+      <c r="C48" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0xB8</v>
+      </c>
+      <c r="D48" s="5">
+        <f t="shared" si="4"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A49" s="5">
+        <f t="shared" si="2"/>
+        <v>188</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>0xBC</v>
+      </c>
+      <c r="C49" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0xBC</v>
+      </c>
+      <c r="D49" s="5">
+        <f t="shared" si="4"/>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A50" s="5">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>0xC0</v>
+      </c>
+      <c r="C50" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0xC0</v>
+      </c>
+      <c r="D50" s="5">
+        <f t="shared" si="4"/>
+        <v>192</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>237</v>
+      </c>
+      <c r="G50" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
-        <f t="shared" si="1"/>
-        <v>184</v>
-      </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>0xB8</v>
-      </c>
-      <c r="C48" s="5" t="str">
-        <f>IF((A48-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A48-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x184</v>
-      </c>
-      <c r="D48" s="5">
-        <f>(A48-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>184</v>
-      </c>
-      <c r="O48" t="s">
+      <c r="H50">
+        <v>44</v>
+      </c>
+      <c r="I50" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A51" s="5">
+        <f t="shared" si="2"/>
+        <v>196</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>0xC4</v>
+      </c>
+      <c r="C51" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0xC4</v>
+      </c>
+      <c r="D51" s="5">
+        <f t="shared" si="4"/>
+        <v>196</v>
+      </c>
+      <c r="E51" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" t="s">
+        <v>238</v>
+      </c>
+      <c r="G51" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
-        <f t="shared" si="1"/>
-        <v>188</v>
-      </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>0xBC</v>
-      </c>
-      <c r="C49" s="5" t="str">
-        <f>IF((A49-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A49-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x188</v>
-      </c>
-      <c r="D49" s="5">
-        <f>(A49-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>188</v>
-      </c>
-      <c r="O49" t="s">
+      <c r="H51">
+        <v>45</v>
+      </c>
+      <c r="I51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A52" s="5">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>0xC8</v>
+      </c>
+      <c r="C52" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0xC8</v>
+      </c>
+      <c r="D52" s="5">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="O52" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
-        <f t="shared" si="1"/>
-        <v>192</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>0xC0</v>
-      </c>
-      <c r="C50" s="5" t="str">
-        <f>IF((A50-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A50-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x192</v>
-      </c>
-      <c r="D50" s="5">
-        <f>(A50-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>192</v>
-      </c>
-      <c r="O50" t="s">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A53" s="5">
+        <f t="shared" si="2"/>
+        <v>204</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>0xCC</v>
+      </c>
+      <c r="C53" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0xCC</v>
+      </c>
+      <c r="D53" s="5">
+        <f t="shared" si="4"/>
+        <v>204</v>
+      </c>
+      <c r="O53" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
-        <f t="shared" si="1"/>
-        <v>196</v>
-      </c>
-      <c r="B51" t="str">
-        <f t="shared" si="0"/>
-        <v>0xC4</v>
-      </c>
-      <c r="C51" s="5" t="str">
-        <f>IF((A51-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A51-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x196</v>
-      </c>
-      <c r="D51" s="5">
-        <f>(A51-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>196</v>
-      </c>
-      <c r="O51" t="s">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A54" s="5">
+        <f t="shared" si="2"/>
+        <v>208</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>0xD0</v>
+      </c>
+      <c r="C54" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0xD0</v>
+      </c>
+      <c r="D54" s="5">
+        <f t="shared" si="4"/>
+        <v>208</v>
+      </c>
+      <c r="O54" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
-        <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>0xC8</v>
-      </c>
-      <c r="C52" s="5" t="str">
-        <f>IF((A52-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A52-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x200</v>
-      </c>
-      <c r="D52" s="5">
-        <f>(A52-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>200</v>
-      </c>
-      <c r="O52" t="s">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A55" s="5">
+        <f t="shared" si="2"/>
+        <v>212</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>0xD4</v>
+      </c>
+      <c r="C55" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0xD4</v>
+      </c>
+      <c r="D55" s="5">
+        <f t="shared" si="4"/>
+        <v>212</v>
+      </c>
+      <c r="O55" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
-        <f t="shared" si="1"/>
-        <v>204</v>
-      </c>
-      <c r="B53" t="str">
-        <f t="shared" si="0"/>
-        <v>0xCC</v>
-      </c>
-      <c r="C53" s="5" t="str">
-        <f>IF((A53-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A53-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x204</v>
-      </c>
-      <c r="D53" s="5">
-        <f>(A53-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>204</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
-        <f t="shared" si="1"/>
-        <v>208</v>
-      </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>0xD0</v>
-      </c>
-      <c r="C54" s="5" t="str">
-        <f>IF((A54-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A54-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x208</v>
-      </c>
-      <c r="D54" s="5">
-        <f>(A54-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>208</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
-        <f t="shared" si="1"/>
-        <v>212</v>
-      </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>0xD4</v>
-      </c>
-      <c r="C55" s="5" t="str">
-        <f>IF((A55-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A55-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x212</v>
-      </c>
-      <c r="D55" s="5">
-        <f>(A55-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>212</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="B56" t="str">
@@ -2448,17 +2520,17 @@
         <v>0xD8</v>
       </c>
       <c r="C56" s="5" t="str">
-        <f>IF((A56-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A56-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x216</v>
+        <f t="shared" si="3"/>
+        <v>0xD8</v>
       </c>
       <c r="D56" s="5">
-        <f>(A56-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
       <c r="B57" t="str">
@@ -2466,17 +2538,17 @@
         <v>0xDC</v>
       </c>
       <c r="C57" s="5" t="str">
-        <f>IF((A57-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A57-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x220</v>
+        <f t="shared" si="3"/>
+        <v>0xDC</v>
       </c>
       <c r="D57" s="5">
-        <f>(A57-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>220</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>224</v>
       </c>
       <c r="B58" t="str">
@@ -2484,17 +2556,17 @@
         <v>0xE0</v>
       </c>
       <c r="C58" s="5" t="str">
-        <f>IF((A58-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A58-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x224</v>
+        <f t="shared" si="3"/>
+        <v>0xE0</v>
       </c>
       <c r="D58" s="5">
-        <f>(A58-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>228</v>
       </c>
       <c r="B59" t="str">
@@ -2502,65 +2574,65 @@
         <v>0xE4</v>
       </c>
       <c r="C59" s="5" t="str">
-        <f>IF((A59-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A59-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x228</v>
+        <f t="shared" si="3"/>
+        <v>0xE4</v>
       </c>
       <c r="D59" s="5">
-        <f>(A59-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
-        <f t="shared" ref="A60:A70" si="2">A59+4</f>
+        <f t="shared" ref="A60:A70" si="5">A59+4</f>
         <v>232</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" ref="B60:B70" si="3">"0x"&amp;DEC2HEX(A60)</f>
+        <f t="shared" ref="B60:B70" si="6">"0x"&amp;DEC2HEX(A60)</f>
         <v>0xE8</v>
       </c>
       <c r="C60" s="5" t="str">
-        <f>IF((A60-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A60-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x232</v>
+        <f t="shared" si="3"/>
+        <v>0xE8</v>
       </c>
       <c r="D60" s="5">
-        <f>(A60-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>232</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>236</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0xEC</v>
       </c>
       <c r="C61" s="5" t="str">
-        <f>IF((A61-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A61-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x236</v>
+        <f t="shared" si="3"/>
+        <v>0xEC</v>
       </c>
       <c r="D61" s="5">
-        <f>(A61-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>236</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0xF0</v>
       </c>
       <c r="C62" s="5" t="str">
-        <f>IF((A62-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A62-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x240</v>
+        <f t="shared" si="3"/>
+        <v>0xF0</v>
       </c>
       <c r="D62" s="5">
-        <f>(A62-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="E62" t="s">
@@ -2570,147 +2642,147 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>244</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0xF4</v>
       </c>
       <c r="C63" s="5" t="str">
-        <f>IF((A63-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A63-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x244</v>
+        <f t="shared" si="3"/>
+        <v>0xF4</v>
       </c>
       <c r="D63" s="5">
-        <f>(A63-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>244</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>248</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0xF8</v>
       </c>
       <c r="C64" s="5" t="str">
-        <f>IF((A64-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A64-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x248</v>
+        <f t="shared" si="3"/>
+        <v>0xF8</v>
       </c>
       <c r="D64" s="5">
-        <f>(A64-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>248</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>252</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0xFC</v>
       </c>
       <c r="C65" s="5" t="str">
-        <f>IF((A65-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A65-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x252</v>
+        <f t="shared" si="3"/>
+        <v>0xFC</v>
       </c>
       <c r="D65" s="5">
-        <f>(A65-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>252</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>256</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0x100</v>
       </c>
       <c r="C66" s="5" t="str">
-        <f>IF((A66-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A66-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x256</v>
+        <f t="shared" si="3"/>
+        <v>0x100</v>
       </c>
       <c r="D66" s="5">
-        <f>(A66-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>256</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>260</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0x104</v>
       </c>
       <c r="C67" s="5" t="str">
-        <f>IF((A67-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A67-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x260</v>
+        <f t="shared" ref="C67:C70" si="7">"0x"&amp;DEC2HEX(D67)</f>
+        <v>0x104</v>
       </c>
       <c r="D67" s="5">
-        <f>(A67-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>260</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>264</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0x108</v>
       </c>
       <c r="C68" s="5" t="str">
-        <f>IF((A68-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A68-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x264</v>
+        <f t="shared" si="7"/>
+        <v>0x108</v>
       </c>
       <c r="D68" s="5">
-        <f>(A68-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>264</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>268</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0x10C</v>
       </c>
       <c r="C69" s="5" t="str">
-        <f>IF((A69-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A69-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x268</v>
+        <f t="shared" si="7"/>
+        <v>0x10C</v>
       </c>
       <c r="D69" s="5">
-        <f>(A69-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>272</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0x110</v>
       </c>
       <c r="C70" s="5" t="str">
-        <f>IF((A70-INDEX(A:A,MATCH("player",F:F,0))) &lt; 0,"-","")&amp;"0x"&amp;ABS(A70-INDEX(A:A,MATCH("player",F:F,0)))</f>
-        <v>0x272</v>
+        <f t="shared" si="7"/>
+        <v>0x110</v>
       </c>
       <c r="D70" s="5">
-        <f>(A70-INDEX(A:A,MATCH("player",F:F,0)))</f>
+        <f t="shared" si="4"/>
         <v>272</v>
       </c>
     </row>
@@ -2728,326 +2800,326 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3063,81 +3135,81 @@
       <selection sqref="A1:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3153,146 +3225,146 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3308,151 +3380,151 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3468,166 +3540,166 @@
       <selection sqref="A1:A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>